<commit_message>
Updated BSD - Protokoll
</commit_message>
<xml_diff>
--- a/doc/BSD - Protokoll.xlsx
+++ b/doc/BSD - Protokoll.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Lamprecht Daniel</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Einrichtung Git Hub &amp; Infrastruktur erweitert</t>
+  </si>
+  <si>
+    <t>Erstellung Daten-Klassen, Login- u. MainGUI</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
   <dimension ref="A2:AA40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,10 +930,21 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2">
+        <v>42665</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
       <c r="M13" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Udated BSD Status doc
</commit_message>
<xml_diff>
--- a/doc/BSD - Protokoll.xlsx
+++ b/doc/BSD - Protokoll.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>Lamprecht Daniel</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t xml:space="preserve">Sprint Meeting </t>
+  </si>
+  <si>
+    <t>Sprint Planning Meeting Sprint 3</t>
+  </si>
+  <si>
+    <t>22.202.2017</t>
   </si>
 </sst>
 </file>
@@ -287,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -330,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27:AA27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1885,10 +1894,21 @@
       <c r="Q28" s="5">
         <v>1</v>
       </c>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="5"/>
+      <c r="W28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="AA28" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
@@ -2034,21 +2054,43 @@
       <c r="Z32" s="4"/>
       <c r="AA32" s="5"/>
     </row>
-    <row r="33" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D33" s="3"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="5"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="5"/>
+    <row r="33" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="P33" s="4">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>1</v>
+      </c>
       <c r="X33" s="3"/>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
       <c r="AA33" s="5"/>
     </row>
-    <row r="34" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2062,7 +2104,7 @@
       <c r="Z34" s="4"/>
       <c r="AA34" s="5"/>
     </row>
-    <row r="35" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2076,7 +2118,7 @@
       <c r="Z35" s="4"/>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2090,7 +2132,7 @@
       <c r="Z36" s="4"/>
       <c r="AA36" s="5"/>
     </row>
-    <row r="37" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -2104,7 +2146,7 @@
       <c r="Z37" s="4"/>
       <c r="AA37" s="5"/>
     </row>
-    <row r="38" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2118,7 +2160,7 @@
       <c r="Z38" s="4"/>
       <c r="AA38" s="5"/>
     </row>
-    <row r="39" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -2132,7 +2174,7 @@
       <c r="Z39" s="4"/>
       <c r="AA39" s="5"/>
     </row>
-    <row r="40" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:27" x14ac:dyDescent="0.3">
       <c r="N40" s="3"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
@@ -2142,7 +2184,7 @@
       <c r="Z40" s="4"/>
       <c r="AA40" s="5"/>
     </row>
-    <row r="42" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:27" x14ac:dyDescent="0.3">
       <c r="M42" s="10" t="s">
         <v>45</v>
       </c>
@@ -2153,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:27" x14ac:dyDescent="0.3">
       <c r="M43" s="6" t="s">
         <v>46</v>
       </c>

</xml_diff>